<commit_message>
Se aplica el patron de diseño Singleton y Chain Of Responsability
</commit_message>
<xml_diff>
--- a/reservas.xlsx
+++ b/reservas.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="16">
   <si>
     <t>Cliente</t>
   </si>
@@ -56,6 +56,18 @@
   </si>
   <si>
     <t>880.0</t>
+  </si>
+  <si>
+    <t>Finca Bella Vista</t>
+  </si>
+  <si>
+    <t>2025-02-02</t>
+  </si>
+  <si>
+    <t>2025-02-05</t>
+  </si>
+  <si>
+    <t>2475.0</t>
   </si>
 </sst>
 </file>
@@ -408,7 +420,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I28" sqref="I28"/>
@@ -433,6 +445,23 @@
         <v>10</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>